<commit_message>
add proper working files to dispatcher
</commit_message>
<xml_diff>
--- a/P2_Dispatcher/Data/Config.xlsx
+++ b/P2_Dispatcher/Data/Config.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andreea.ghetu\Documents\UiPath\CSharpChanges\StudioTemplates\REFramework\C#\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96902286-4E3C-425E-A0BF-F83C72A8C5F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="18000" windowHeight="9480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1176" yWindow="1176" windowWidth="18000" windowHeight="9480"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -88,10 +82,6 @@
   </si>
   <si>
     <t>Framework</t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -161,12 +151,18 @@
   </si>
   <si>
     <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>GetawayGurus</t>
+  </si>
+  <si>
+    <t>tripQueue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -533,29 +529,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18.75">
+    <row r="1" spans="1:26" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,27 +587,30 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="45">
+    </row>
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -619,7 +618,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -630,22 +629,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18.75">
+    <row r="1" spans="1:26" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -679,7 +678,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -687,18 +686,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="5">
         <v>0</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -725,7 +724,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -747,7 +746,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -758,7 +757,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -769,18 +768,18 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:26">
@@ -790,35 +789,35 @@
     </row>
     <row r="14" spans="1:26">
       <c r="A14" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="5">
         <v>2</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="5">
         <v>2</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="5" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -828,19 +827,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -851,7 +850,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
fix reframework to not use orchestrator
</commit_message>
<xml_diff>
--- a/P2_Dispatcher/Data/Config.xlsx
+++ b/P2_Dispatcher/Data/Config.xlsx
@@ -81,21 +81,10 @@
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
-    <t>Framework</t>
-  </si>
-  <si>
-    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
   </si>
   <si>
@@ -132,9 +121,6 @@
     <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
   </si>
   <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
     <t>ShouldMarkJobAsFaulted</t>
   </si>
   <si>
@@ -150,13 +136,25 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>GetawayGurus</t>
-  </si>
-  <si>
-    <t>tripQueue</t>
+    <t>P2Dispatcher</t>
+  </si>
+  <si>
+    <t>SampleDataFolder</t>
+  </si>
+  <si>
+    <t>Folder name for customer data.</t>
+  </si>
+  <si>
+    <t>MyEmail</t>
+  </si>
+  <si>
+    <t>goombaxl23xl@gmail.com</t>
+  </si>
+  <si>
+    <t>Email for sending outgoing stuff to customers, as well as getting the initial travel plans.</t>
+  </si>
+  <si>
+    <t>..\\customerqueue\\</t>
   </si>
 </sst>
 </file>
@@ -529,7 +527,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -537,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -585,40 +583,37 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26">
-      <c r="A2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:26" ht="28.8">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="43.2">
-      <c r="A3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
+      <c r="A4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
         <v>44</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26">
-      <c r="A4" s="7"/>
-    </row>
-    <row r="5" spans="1:26" ht="28.8">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -686,18 +681,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B3" s="5">
         <v>0</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -724,7 +719,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -746,7 +741,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -757,7 +752,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -768,18 +763,18 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:26">
@@ -789,35 +784,35 @@
     </row>
     <row r="14" spans="1:26">
       <c r="A14" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B14" s="5">
         <v>2</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B15" s="5">
         <v>2</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="28.8">
       <c r="A17" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B17" s="5" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -850,7 +845,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>